<commit_message>
feat(Issue #1): 完善了 TopBanner 组件。
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="225">
   <si>
     <t>序号</t>
   </si>
@@ -683,6 +683,12 @@
   </si>
   <si>
     <t>身份认证</t>
+  </si>
+  <si>
+    <t>Application_Name</t>
+  </si>
+  <si>
+    <t>.NET &amp; Vue</t>
   </si>
 </sst>
 </file>
@@ -690,10 +696,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -724,16 +730,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -746,6 +744,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -753,8 +804,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -770,14 +822,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -786,16 +830,17 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -808,39 +853,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -848,14 +862,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -877,7 +883,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -889,13 +943,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -907,19 +1003,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,133 +1063,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1086,6 +1092,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1097,6 +1121,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1120,40 +1159,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1176,10 +1182,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1188,133 +1194,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1653,10 +1659,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+      <selection activeCell="F108" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -2735,14 +2741,14 @@
         <v>107</v>
       </c>
       <c r="D49" s="2" t="str">
-        <f t="shared" ref="D49:D54" si="6">UPPER(B49)&amp;": """&amp;C49&amp;""","</f>
+        <f t="shared" ref="D49:D58" si="6">UPPER(B49)&amp;": """&amp;C49&amp;""","</f>
         <v>QQ: "QQ",</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>108</v>
       </c>
       <c r="F49" s="2" t="str">
-        <f t="shared" ref="F49:F54" si="7">UPPER(B49)&amp;": """&amp;E49&amp;""","</f>
+        <f t="shared" ref="F49:F58" si="7">UPPER(B49)&amp;": """&amp;E49&amp;""","</f>
         <v>QQ: "Tencent QQ",</v>
       </c>
     </row>
@@ -2867,14 +2873,14 @@
         <v>4</v>
       </c>
       <c r="D55" s="2" t="str">
-        <f>UPPER(B55)&amp;": """&amp;C55&amp;""","</f>
+        <f t="shared" si="6"/>
         <v>ENGLISH_USA: "英语（美国）",</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F55" s="2" t="str">
-        <f>UPPER(B55)&amp;": """&amp;E55&amp;""","</f>
+        <f t="shared" si="7"/>
         <v>ENGLISH_USA: "USA",</v>
       </c>
     </row>
@@ -2889,14 +2895,14 @@
         <v>124</v>
       </c>
       <c r="D56" s="2" t="str">
-        <f>UPPER(B56)&amp;": """&amp;C56&amp;""","</f>
+        <f t="shared" si="6"/>
         <v>SUBMIT: "提交",</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>123</v>
       </c>
       <c r="F56" s="2" t="str">
-        <f>UPPER(B56)&amp;": """&amp;E56&amp;""","</f>
+        <f t="shared" si="7"/>
         <v>SUBMIT: "Submit",</v>
       </c>
     </row>
@@ -2911,14 +2917,14 @@
         <v>126</v>
       </c>
       <c r="D57" s="2" t="str">
-        <f>UPPER(B57)&amp;": """&amp;C57&amp;""","</f>
+        <f t="shared" si="6"/>
         <v>RESET: "重置",</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>125</v>
       </c>
       <c r="F57" s="2" t="str">
-        <f>UPPER(B57)&amp;": """&amp;E57&amp;""","</f>
+        <f t="shared" si="7"/>
         <v>RESET: "Reset",</v>
       </c>
     </row>
@@ -2933,14 +2939,14 @@
         <v>128</v>
       </c>
       <c r="D58" s="2" t="str">
-        <f>UPPER(B58)&amp;": """&amp;C58&amp;""","</f>
+        <f t="shared" si="6"/>
         <v>CONFIGURATION: "配置",</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>127</v>
       </c>
       <c r="F58" s="2" t="str">
-        <f>UPPER(B58)&amp;": """&amp;E58&amp;""","</f>
+        <f t="shared" si="7"/>
         <v>CONFIGURATION: "Configuration",</v>
       </c>
     </row>
@@ -2955,14 +2961,14 @@
         <v>130</v>
       </c>
       <c r="D59" s="2" t="str">
-        <f t="shared" ref="D59:D65" si="8">UPPER(B59)&amp;": """&amp;C59&amp;""","</f>
+        <f t="shared" ref="D59:D69" si="8">UPPER(B59)&amp;": """&amp;C59&amp;""","</f>
         <v>SETTINGS: "设置",</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F59" s="2" t="str">
-        <f t="shared" ref="F59:F65" si="9">UPPER(B59)&amp;": """&amp;E59&amp;""","</f>
+        <f t="shared" ref="F59:F69" si="9">UPPER(B59)&amp;": """&amp;E59&amp;""","</f>
         <v>SETTINGS: "Settings",</v>
       </c>
     </row>
@@ -3109,14 +3115,14 @@
         <v>149</v>
       </c>
       <c r="D66" s="2" t="str">
-        <f>UPPER(B66)&amp;": """&amp;C66&amp;""","</f>
+        <f t="shared" si="8"/>
         <v>PAUSE: "暂停",</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F66" s="2" t="str">
-        <f>UPPER(B66)&amp;": """&amp;E66&amp;""","</f>
+        <f t="shared" si="9"/>
         <v>PAUSE: "Pause",</v>
       </c>
     </row>
@@ -3131,14 +3137,14 @@
         <v>151</v>
       </c>
       <c r="D67" s="2" t="str">
-        <f>UPPER(B67)&amp;": """&amp;C67&amp;""","</f>
+        <f t="shared" si="8"/>
         <v>ABORT: "终止",</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>150</v>
       </c>
       <c r="F67" s="2" t="str">
-        <f>UPPER(B67)&amp;": """&amp;E67&amp;""","</f>
+        <f t="shared" si="9"/>
         <v>ABORT: "Abort",</v>
       </c>
     </row>
@@ -3153,14 +3159,14 @@
         <v>153</v>
       </c>
       <c r="D68" s="2" t="str">
-        <f>UPPER(B68)&amp;": """&amp;C68&amp;""","</f>
+        <f t="shared" si="8"/>
         <v>UPLOAD: "上传",</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>152</v>
       </c>
       <c r="F68" s="2" t="str">
-        <f>UPPER(B68)&amp;": """&amp;E68&amp;""","</f>
+        <f t="shared" si="9"/>
         <v>UPLOAD: "Upload",</v>
       </c>
     </row>
@@ -3175,14 +3181,14 @@
         <v>155</v>
       </c>
       <c r="D69" s="2" t="str">
-        <f>UPPER(B69)&amp;": """&amp;C69&amp;""","</f>
+        <f t="shared" si="8"/>
         <v>DOWNLOAD: "下载",</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>154</v>
       </c>
       <c r="F69" s="2" t="str">
-        <f>UPPER(B69)&amp;": """&amp;E69&amp;""","</f>
+        <f t="shared" si="9"/>
         <v>DOWNLOAD: "Download",</v>
       </c>
     </row>
@@ -3888,6 +3894,28 @@
       <c r="F101" s="2" t="str">
         <f t="shared" si="15"/>
         <v>AUTHENTICATE: "Authenticate",</v>
+      </c>
+    </row>
+    <row r="102" customHeight="1" spans="1:6">
+      <c r="A102" s="4">
+        <v>101</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D102" s="2" t="str">
+        <f>UPPER(B102)&amp;": """&amp;C102&amp;""","</f>
+        <v>APPLICATION_NAME: ".NET &amp; Vue",</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F102" s="2" t="str">
+        <f>UPPER(B102)&amp;": """&amp;E102&amp;""","</f>
+        <v>APPLICATION_NAME: ".NET &amp; Vue",</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Issue #9): 新增 SafeNumber 和组合式 API。
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -10,7 +10,7 @@
     <sheet name="默认多语言资源" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$104</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -717,10 +717,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -751,8 +751,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -765,9 +788,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,60 +833,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -850,24 +850,24 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -904,7 +904,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,61 +1018,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,25 +1030,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,19 +1048,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,43 +1072,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1095,30 +1095,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1146,6 +1122,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1161,17 +1152,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1181,6 +1166,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1203,10 +1203,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1215,133 +1215,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1683,19 +1683,19 @@
   <dimension ref="A1:F104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B106" sqref="B106"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="$A105:$XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
-    <col min="2" max="2" width="18.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="32.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="43.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="63.25" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -3754,14 +3754,14 @@
         <v>202</v>
       </c>
       <c r="D94" s="2" t="str">
-        <f t="shared" ref="D94:D101" si="14">UPPER(B94)&amp;": """&amp;C94&amp;""","</f>
+        <f t="shared" ref="D94:D104" si="14">UPPER(B94)&amp;": """&amp;C94&amp;""","</f>
         <v>OFFICIAL_SITE: "官网",</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F94" s="2" t="str">
-        <f t="shared" ref="F94:F101" si="15">UPPER(B94)&amp;": """&amp;E94&amp;""","</f>
+        <f t="shared" ref="F94:F104" si="15">UPPER(B94)&amp;": """&amp;E94&amp;""","</f>
         <v>OFFICIAL_SITE: "Official Site",</v>
       </c>
     </row>
@@ -3930,14 +3930,14 @@
         <v>224</v>
       </c>
       <c r="D102" s="2" t="str">
-        <f>UPPER(B102)&amp;": """&amp;C102&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>APPLICATION_NAME: ".NET &amp; Vue",</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>224</v>
       </c>
       <c r="F102" s="2" t="str">
-        <f>UPPER(B102)&amp;": """&amp;E102&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>APPLICATION_NAME: ".NET &amp; Vue",</v>
       </c>
     </row>
@@ -3952,14 +3952,14 @@
         <v>226</v>
       </c>
       <c r="D103" s="2" t="str">
-        <f>UPPER(B103)&amp;": """&amp;C103&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>CONTROL_PANEL: "控制面板",</v>
       </c>
       <c r="E103" s="2" t="s">
         <v>227</v>
       </c>
       <c r="F103" s="2" t="str">
-        <f>UPPER(B103)&amp;": """&amp;E103&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>CONTROL_PANEL: "Control Panel",</v>
       </c>
     </row>
@@ -3974,19 +3974,19 @@
         <v>229</v>
       </c>
       <c r="D104" s="2" t="str">
-        <f>UPPER(B104)&amp;": """&amp;C104&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>APPLICATION_MANIFEST: "应用清单",</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>230</v>
       </c>
       <c r="F104" s="2" t="str">
-        <f>UPPER(B104)&amp;": """&amp;E104&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>APPLICATION_MANIFEST: "Application Manifest",</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F103">
+  <autoFilter ref="A1:F104">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(Issue #14): 调整了 IAuthenticationService 接口定义。
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="234">
   <si>
     <t>序号</t>
   </si>
@@ -710,6 +710,15 @@
   </si>
   <si>
     <t>Application Manifest</t>
+  </si>
+  <si>
+    <t>Invalid_Credentials</t>
+  </si>
+  <si>
+    <t>必须提供用户名和登录密码。</t>
+  </si>
+  <si>
+    <t>The username and login password must be provided.</t>
   </si>
 </sst>
 </file>
@@ -718,8 +727,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -751,16 +760,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -768,6 +776,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -781,45 +811,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -835,15 +829,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -857,6 +858,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -866,8 +881,16 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -875,21 +898,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -904,7 +913,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -916,7 +1021,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -928,13 +1039,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,73 +1075,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1024,67 +1093,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1095,15 +1104,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1123,6 +1123,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -1133,6 +1148,44 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1151,50 +1204,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1203,10 +1212,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1215,133 +1224,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1680,12 +1689,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="$A105:$XFD105"/>
+      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -1694,7 +1703,7 @@
     <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="57.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.375" style="2" customWidth="1"/>
     <col min="6" max="6" width="63.25" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
@@ -3983,6 +3992,28 @@
       <c r="F104" s="2" t="str">
         <f t="shared" si="15"/>
         <v>APPLICATION_MANIFEST: "Application Manifest",</v>
+      </c>
+    </row>
+    <row r="105" customHeight="1" spans="1:6">
+      <c r="A105" s="4">
+        <v>104</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D105" s="2" t="str">
+        <f>UPPER(B105)&amp;": """&amp;C105&amp;""","</f>
+        <v>INVALID_CREDENTIALS: "必须提供用户名和登录密码。",</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F105" s="2" t="str">
+        <f>UPPER(B105)&amp;": """&amp;E105&amp;""","</f>
+        <v>INVALID_CREDENTIALS: "The username and login password must be provided.",</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(Issue #15): 新增 v-toolbar.vue 组件。
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -10,14 +10,14 @@
     <sheet name="默认多语言资源" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$110</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="251">
   <si>
     <t>序号</t>
   </si>
@@ -752,6 +752,24 @@
   </si>
   <si>
     <t>请输入登录密码</t>
+  </si>
+  <si>
+    <t>Current_User</t>
+  </si>
+  <si>
+    <t>当前用户</t>
+  </si>
+  <si>
+    <t>The user</t>
+  </si>
+  <si>
+    <t>Change_Password</t>
+  </si>
+  <si>
+    <t>修改登录密码</t>
+  </si>
+  <si>
+    <t>Change my password</t>
   </si>
 </sst>
 </file>
@@ -760,9 +778,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -795,14 +813,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -823,36 +841,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -866,14 +855,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -882,11 +863,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -915,6 +895,29 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -930,8 +933,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -946,7 +964,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -958,175 +1144,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1140,17 +1158,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1187,17 +1199,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -1205,11 +1206,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1231,6 +1238,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1245,10 +1263,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1257,133 +1275,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1722,12 +1740,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F109"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
+      <selection pane="bottomLeft" activeCell="F111" sqref="F111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -3796,14 +3814,14 @@
         <v>202</v>
       </c>
       <c r="D94" s="2" t="str">
-        <f t="shared" ref="D94:D106" si="14">UPPER(B94)&amp;": """&amp;C94&amp;""","</f>
+        <f t="shared" ref="D94:D109" si="14">UPPER(B94)&amp;": """&amp;C94&amp;""","</f>
         <v>OFFICIAL_SITE: "官网",</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F94" s="2" t="str">
-        <f t="shared" ref="F94:F106" si="15">UPPER(B94)&amp;": """&amp;E94&amp;""","</f>
+        <f t="shared" ref="F94:F109" si="15">UPPER(B94)&amp;": """&amp;E94&amp;""","</f>
         <v>OFFICIAL_SITE: "Official Site",</v>
       </c>
     </row>
@@ -4082,14 +4100,14 @@
         <v>238</v>
       </c>
       <c r="D107" s="2" t="str">
-        <f>UPPER(B107)&amp;": """&amp;C107&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>AUTHENTICATION_IN_PROGRESS: "身份认证中，请稍候...",</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>239</v>
       </c>
       <c r="F107" s="2" t="str">
-        <f>UPPER(B107)&amp;": """&amp;E107&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>AUTHENTICATION_IN_PROGRESS: "Authentication in progress, please wait",</v>
       </c>
     </row>
@@ -4104,14 +4122,14 @@
         <v>241</v>
       </c>
       <c r="D108" s="2" t="str">
-        <f>UPPER(B108)&amp;": """&amp;C108&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>ENTER_USERNAME: "请输入用户名 / 电邮地址 / 手机号",</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>242</v>
       </c>
       <c r="F108" s="2" t="str">
-        <f>UPPER(B108)&amp;": """&amp;E108&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>ENTER_USERNAME: "User Name / E-mail Address / Mobile Number",</v>
       </c>
     </row>
@@ -4126,19 +4144,63 @@
         <v>244</v>
       </c>
       <c r="D109" s="2" t="str">
-        <f>UPPER(B109)&amp;": """&amp;C109&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>ENTER_PASSWORD: "请输入登录密码",</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>216</v>
       </c>
       <c r="F109" s="2" t="str">
-        <f>UPPER(B109)&amp;": """&amp;E109&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>ENTER_PASSWORD: "Password",</v>
       </c>
     </row>
+    <row r="110" customHeight="1" spans="1:6">
+      <c r="A110" s="4">
+        <v>109</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D110" s="2" t="str">
+        <f>UPPER(B110)&amp;": """&amp;C110&amp;""","</f>
+        <v>CURRENT_USER: "当前用户",</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F110" s="2" t="str">
+        <f>UPPER(B110)&amp;": """&amp;E110&amp;""","</f>
+        <v>CURRENT_USER: "The user",</v>
+      </c>
+    </row>
+    <row r="111" customHeight="1" spans="1:6">
+      <c r="A111" s="4">
+        <v>110</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D111" s="2" t="str">
+        <f>UPPER(B111)&amp;": """&amp;C111&amp;""","</f>
+        <v>CHANGE_PASSWORD: "修改登录密码",</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F111" s="2" t="str">
+        <f>UPPER(B111)&amp;": """&amp;E111&amp;""","</f>
+        <v>CHANGE_PASSWORD: "Change my password",</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F106">
+  <autoFilter ref="A1:F110">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(Issue #16): 重启 Issues #16
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -10,14 +10,14 @@
     <sheet name="默认多语言资源" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$111</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$112</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="254">
   <si>
     <t>序号</t>
   </si>
@@ -770,6 +770,15 @@
   </si>
   <si>
     <t>Change my password</t>
+  </si>
+  <si>
+    <t>Home_Page</t>
+  </si>
+  <si>
+    <t>首页</t>
+  </si>
+  <si>
+    <t>Home</t>
   </si>
 </sst>
 </file>
@@ -1739,13 +1748,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F111"/>
+  <sheetPr/>
+  <dimension ref="A1:F112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <selection pane="bottomLeft" activeCell="G111" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -1779,7 +1788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" hidden="1" customHeight="1" spans="1:6">
+    <row r="2" customHeight="1" spans="1:6">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1801,7 +1810,7 @@
         <v>DEBUG: "Debug",</v>
       </c>
     </row>
-    <row r="3" hidden="1" customHeight="1" spans="1:6">
+    <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>TRACE: "Trace",</v>
       </c>
     </row>
-    <row r="4" hidden="1" customHeight="1" spans="1:6">
+    <row r="4" customHeight="1" spans="1:6">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1845,7 +1854,7 @@
         <v>INFORMATION: "Information",</v>
       </c>
     </row>
-    <row r="5" hidden="1" customHeight="1" spans="1:6">
+    <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>WARNING: "Warning",</v>
       </c>
     </row>
-    <row r="6" hidden="1" customHeight="1" spans="1:6">
+    <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1911,7 +1920,7 @@
         <v>EXCEPTION: "Exception",</v>
       </c>
     </row>
-    <row r="8" hidden="1" customHeight="1" spans="1:6">
+    <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>FATAL: "Fatal",</v>
       </c>
     </row>
-    <row r="9" hidden="1" customHeight="1" spans="1:6">
+    <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1955,7 +1964,7 @@
         <v>DANGEROUS: "Dangerous",</v>
       </c>
     </row>
-    <row r="10" hidden="1" customHeight="1" spans="1:6">
+    <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1977,7 +1986,7 @@
         <v>OK: "Ok",</v>
       </c>
     </row>
-    <row r="11" hidden="1" customHeight="1" spans="1:6">
+    <row r="11" customHeight="1" spans="1:6">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1999,7 +2008,7 @@
         <v>CANCEL: "Cancel",</v>
       </c>
     </row>
-    <row r="12" hidden="1" customHeight="1" spans="1:6">
+    <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>SUCCESS: "Success",</v>
       </c>
     </row>
-    <row r="13" hidden="1" customHeight="1" spans="1:6">
+    <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2043,7 +2052,7 @@
         <v>FAILED: "Failed",</v>
       </c>
     </row>
-    <row r="14" hidden="1" customHeight="1" spans="1:6">
+    <row r="14" customHeight="1" spans="1:6">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2065,7 +2074,7 @@
         <v>COMPLETED: "Is Completed",</v>
       </c>
     </row>
-    <row r="15" hidden="1" customHeight="1" spans="1:6">
+    <row r="15" customHeight="1" spans="1:6">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2087,7 +2096,7 @@
         <v>DONE: "Is Done",</v>
       </c>
     </row>
-    <row r="16" hidden="1" customHeight="1" spans="1:6">
+    <row r="16" customHeight="1" spans="1:6">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2109,7 +2118,7 @@
         <v>CREATE_NEW: "New",</v>
       </c>
     </row>
-    <row r="17" hidden="1" customHeight="1" spans="1:6">
+    <row r="17" customHeight="1" spans="1:6">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2131,7 +2140,7 @@
         <v>EDIT: "Edit",</v>
       </c>
     </row>
-    <row r="18" hidden="1" customHeight="1" spans="1:6">
+    <row r="18" customHeight="1" spans="1:6">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2153,7 +2162,7 @@
         <v>SAVE: "Save",</v>
       </c>
     </row>
-    <row r="19" hidden="1" customHeight="1" spans="1:6">
+    <row r="19" customHeight="1" spans="1:6">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2175,7 +2184,7 @@
         <v>SAVE_AS: "Save As",</v>
       </c>
     </row>
-    <row r="20" hidden="1" customHeight="1" spans="1:6">
+    <row r="20" customHeight="1" spans="1:6">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2197,7 +2206,7 @@
         <v>START: "Start",</v>
       </c>
     </row>
-    <row r="21" hidden="1" customHeight="1" spans="1:6">
+    <row r="21" customHeight="1" spans="1:6">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2219,7 +2228,7 @@
         <v>STOP: "Stop",</v>
       </c>
     </row>
-    <row r="22" hidden="1" customHeight="1" spans="1:6">
+    <row r="22" customHeight="1" spans="1:6">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2241,7 +2250,7 @@
         <v>BEGIN: "Begin",</v>
       </c>
     </row>
-    <row r="23" hidden="1" customHeight="1" spans="1:6">
+    <row r="23" customHeight="1" spans="1:6">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2263,7 +2272,7 @@
         <v>START_UP: "Start Up",</v>
       </c>
     </row>
-    <row r="24" hidden="1" customHeight="1" spans="1:6">
+    <row r="24" customHeight="1" spans="1:6">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2285,7 +2294,7 @@
         <v>RUN: "Run",</v>
       </c>
     </row>
-    <row r="25" hidden="1" customHeight="1" spans="1:6">
+    <row r="25" customHeight="1" spans="1:6">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2307,7 +2316,7 @@
         <v>RUNNING: "Running",</v>
       </c>
     </row>
-    <row r="26" hidden="1" customHeight="1" spans="1:6">
+    <row r="26" customHeight="1" spans="1:6">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>COPY: "Copy",</v>
       </c>
     </row>
-    <row r="27" hidden="1" customHeight="1" spans="1:6">
+    <row r="27" customHeight="1" spans="1:6">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2351,7 +2360,7 @@
         <v>PASTE: "Paste",</v>
       </c>
     </row>
-    <row r="28" hidden="1" customHeight="1" spans="1:6">
+    <row r="28" customHeight="1" spans="1:6">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2373,7 +2382,7 @@
         <v>CUT: "Cut",</v>
       </c>
     </row>
-    <row r="29" hidden="1" customHeight="1" spans="1:6">
+    <row r="29" customHeight="1" spans="1:6">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2395,7 +2404,7 @@
         <v>QUERY: "Query",</v>
       </c>
     </row>
-    <row r="30" hidden="1" customHeight="1" spans="1:6">
+    <row r="30" customHeight="1" spans="1:6">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2417,7 +2426,7 @@
         <v>SEARCH: "Search",</v>
       </c>
     </row>
-    <row r="31" hidden="1" customHeight="1" spans="1:6">
+    <row r="31" customHeight="1" spans="1:6">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2439,7 +2448,7 @@
         <v>ADVANCED_QUERY: "Advanced Query",</v>
       </c>
     </row>
-    <row r="32" hidden="1" customHeight="1" spans="1:6">
+    <row r="32" customHeight="1" spans="1:6">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2461,7 +2470,7 @@
         <v>ADVANCED_SEARCH: "Advanced Search",</v>
       </c>
     </row>
-    <row r="33" hidden="1" customHeight="1" spans="1:6">
+    <row r="33" customHeight="1" spans="1:6">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2483,7 +2492,7 @@
         <v>DELETE: "Delete",</v>
       </c>
     </row>
-    <row r="34" hidden="1" customHeight="1" spans="1:6">
+    <row r="34" customHeight="1" spans="1:6">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2505,7 +2514,7 @@
         <v>REMOVE: "Remove",</v>
       </c>
     </row>
-    <row r="35" hidden="1" customHeight="1" spans="1:6">
+    <row r="35" customHeight="1" spans="1:6">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -2527,7 +2536,7 @@
         <v>DISABLE: "Disable",</v>
       </c>
     </row>
-    <row r="36" hidden="1" customHeight="1" spans="1:6">
+    <row r="36" customHeight="1" spans="1:6">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -2549,7 +2558,7 @@
         <v>RESTORE: "Restore",</v>
       </c>
     </row>
-    <row r="37" hidden="1" customHeight="1" spans="1:6">
+    <row r="37" customHeight="1" spans="1:6">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2571,7 +2580,7 @@
         <v>NORMAL: "Normal",</v>
       </c>
     </row>
-    <row r="38" hidden="1" customHeight="1" spans="1:6">
+    <row r="38" customHeight="1" spans="1:6">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -2593,7 +2602,7 @@
         <v>DELETED: "Is Deleted",</v>
       </c>
     </row>
-    <row r="39" hidden="1" customHeight="1" spans="1:6">
+    <row r="39" customHeight="1" spans="1:6">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -2615,7 +2624,7 @@
         <v>STATUS: "Status",</v>
       </c>
     </row>
-    <row r="40" hidden="1" customHeight="1" spans="1:6">
+    <row r="40" customHeight="1" spans="1:6">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -2637,7 +2646,7 @@
         <v>APPEND: "Append",</v>
       </c>
     </row>
-    <row r="41" hidden="1" customHeight="1" spans="1:6">
+    <row r="41" customHeight="1" spans="1:6">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -2659,7 +2668,7 @@
         <v>INSERT: "Insert",</v>
       </c>
     </row>
-    <row r="42" hidden="1" customHeight="1" spans="1:6">
+    <row r="42" customHeight="1" spans="1:6">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -2681,7 +2690,7 @@
         <v>NOTIFICATION: "Notification",</v>
       </c>
     </row>
-    <row r="43" hidden="1" customHeight="1" spans="1:6">
+    <row r="43" customHeight="1" spans="1:6">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -2703,7 +2712,7 @@
         <v>PROMPT: "Prompt",</v>
       </c>
     </row>
-    <row r="44" hidden="1" customHeight="1" spans="1:6">
+    <row r="44" customHeight="1" spans="1:6">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -2725,7 +2734,7 @@
         <v>VIEW: "View",</v>
       </c>
     </row>
-    <row r="45" hidden="1" customHeight="1" spans="1:6">
+    <row r="45" customHeight="1" spans="1:6">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -2747,7 +2756,7 @@
         <v>DETAILS: "Details",</v>
       </c>
     </row>
-    <row r="46" hidden="1" customHeight="1" spans="1:6">
+    <row r="46" customHeight="1" spans="1:6">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -2769,7 +2778,7 @@
         <v>PAYMENT: "Payment",</v>
       </c>
     </row>
-    <row r="47" hidden="1" customHeight="1" spans="1:6">
+    <row r="47" customHeight="1" spans="1:6">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2791,7 +2800,7 @@
         <v>WECHAT: "Tencent WeChat",</v>
       </c>
     </row>
-    <row r="48" hidden="1" customHeight="1" spans="1:6">
+    <row r="48" customHeight="1" spans="1:6">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2813,7 +2822,7 @@
         <v>REFRESH: "Refresh",</v>
       </c>
     </row>
-    <row r="49" hidden="1" customHeight="1" spans="1:6">
+    <row r="49" customHeight="1" spans="1:6">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2835,7 +2844,7 @@
         <v>QQ: "Tencent QQ",</v>
       </c>
     </row>
-    <row r="50" hidden="1" customHeight="1" spans="1:6">
+    <row r="50" customHeight="1" spans="1:6">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2857,7 +2866,7 @@
         <v>ZHIFUBAO: "Alibaba Zhifubao",</v>
       </c>
     </row>
-    <row r="51" hidden="1" customHeight="1" spans="1:6">
+    <row r="51" customHeight="1" spans="1:6">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2879,7 +2888,7 @@
         <v>JD: "Jing Dong",</v>
       </c>
     </row>
-    <row r="52" hidden="1" customHeight="1" spans="1:6">
+    <row r="52" customHeight="1" spans="1:6">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -2901,7 +2910,7 @@
         <v>ALIYUN: "Aliyun",</v>
       </c>
     </row>
-    <row r="53" hidden="1" customHeight="1" spans="1:6">
+    <row r="53" customHeight="1" spans="1:6">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2923,7 +2932,7 @@
         <v>LANGUAGE: "Language",</v>
       </c>
     </row>
-    <row r="54" hidden="1" customHeight="1" spans="1:6">
+    <row r="54" customHeight="1" spans="1:6">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -2945,7 +2954,7 @@
         <v>SIMPLIFIED_CHINESE: "Simplified Chinese",</v>
       </c>
     </row>
-    <row r="55" hidden="1" customHeight="1" spans="1:6">
+    <row r="55" customHeight="1" spans="1:6">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>ENGLISH_USA: "USA",</v>
       </c>
     </row>
-    <row r="56" hidden="1" customHeight="1" spans="1:6">
+    <row r="56" customHeight="1" spans="1:6">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -2989,7 +2998,7 @@
         <v>SUBMIT: "Submit",</v>
       </c>
     </row>
-    <row r="57" hidden="1" customHeight="1" spans="1:6">
+    <row r="57" customHeight="1" spans="1:6">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -3011,7 +3020,7 @@
         <v>RESET: "Reset",</v>
       </c>
     </row>
-    <row r="58" hidden="1" customHeight="1" spans="1:6">
+    <row r="58" customHeight="1" spans="1:6">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -3033,7 +3042,7 @@
         <v>CONFIGURATION: "Configuration",</v>
       </c>
     </row>
-    <row r="59" hidden="1" customHeight="1" spans="1:6">
+    <row r="59" customHeight="1" spans="1:6">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -3055,7 +3064,7 @@
         <v>SETTINGS: "Settings",</v>
       </c>
     </row>
-    <row r="60" hidden="1" customHeight="1" spans="1:6">
+    <row r="60" customHeight="1" spans="1:6">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -3077,7 +3086,7 @@
         <v>PROFILE: "Personal Profile",</v>
       </c>
     </row>
-    <row r="61" hidden="1" customHeight="1" spans="1:6">
+    <row r="61" customHeight="1" spans="1:6">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>SECURITY: "Security",</v>
       </c>
     </row>
-    <row r="62" hidden="1" customHeight="1" spans="1:6">
+    <row r="62" customHeight="1" spans="1:6">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -3121,7 +3130,7 @@
         <v>SIGN_IN: "Sign In",</v>
       </c>
     </row>
-    <row r="63" hidden="1" customHeight="1" spans="1:6">
+    <row r="63" customHeight="1" spans="1:6">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -3143,7 +3152,7 @@
         <v>SIGN_OUT: "Sign Out",</v>
       </c>
     </row>
-    <row r="64" hidden="1" customHeight="1" spans="1:6">
+    <row r="64" customHeight="1" spans="1:6">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>SIGN_OFF: "Sign Off",</v>
       </c>
     </row>
-    <row r="65" hidden="1" customHeight="1" spans="1:6">
+    <row r="65" customHeight="1" spans="1:6">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -3187,7 +3196,7 @@
         <v>SIGN_UP: "Sign Up",</v>
       </c>
     </row>
-    <row r="66" hidden="1" customHeight="1" spans="1:6">
+    <row r="66" customHeight="1" spans="1:6">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -3209,7 +3218,7 @@
         <v>PAUSE: "Pause",</v>
       </c>
     </row>
-    <row r="67" hidden="1" customHeight="1" spans="1:6">
+    <row r="67" customHeight="1" spans="1:6">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -3231,7 +3240,7 @@
         <v>ABORT: "Abort",</v>
       </c>
     </row>
-    <row r="68" hidden="1" customHeight="1" spans="1:6">
+    <row r="68" customHeight="1" spans="1:6">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -3253,7 +3262,7 @@
         <v>UPLOAD: "Upload",</v>
       </c>
     </row>
-    <row r="69" hidden="1" customHeight="1" spans="1:6">
+    <row r="69" customHeight="1" spans="1:6">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -3275,7 +3284,7 @@
         <v>DOWNLOAD: "Download",</v>
       </c>
     </row>
-    <row r="70" hidden="1" customHeight="1" spans="1:6">
+    <row r="70" customHeight="1" spans="1:6">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -3297,7 +3306,7 @@
         <v>CLEAN: "Clean",</v>
       </c>
     </row>
-    <row r="71" hidden="1" customHeight="1" spans="1:6">
+    <row r="71" customHeight="1" spans="1:6">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -3341,7 +3350,7 @@
         <v>EXPAND: "Expand",</v>
       </c>
     </row>
-    <row r="73" hidden="1" customHeight="1" spans="1:6">
+    <row r="73" customHeight="1" spans="1:6">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -3363,7 +3372,7 @@
         <v>COLLAPSE: "Collapse",</v>
       </c>
     </row>
-    <row r="74" hidden="1" customHeight="1" spans="1:6">
+    <row r="74" customHeight="1" spans="1:6">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -3385,7 +3394,7 @@
         <v>MORE: "More",</v>
       </c>
     </row>
-    <row r="75" hidden="1" customHeight="1" spans="1:6">
+    <row r="75" customHeight="1" spans="1:6">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v>SEE: "See",</v>
       </c>
     </row>
-    <row r="76" hidden="1" customHeight="1" spans="1:6">
+    <row r="76" customHeight="1" spans="1:6">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -3451,7 +3460,7 @@
         <v>NEXT_PAGE: "Next Page",</v>
       </c>
     </row>
-    <row r="78" hidden="1" customHeight="1" spans="1:6">
+    <row r="78" customHeight="1" spans="1:6">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -3473,7 +3482,7 @@
         <v>MICROSOFT: "Microsoft",</v>
       </c>
     </row>
-    <row r="79" hidden="1" customHeight="1" spans="1:6">
+    <row r="79" customHeight="1" spans="1:6">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -3495,7 +3504,7 @@
         <v>WINDOWS: "Windows",</v>
       </c>
     </row>
-    <row r="80" hidden="1" customHeight="1" spans="1:6">
+    <row r="80" customHeight="1" spans="1:6">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -3517,7 +3526,7 @@
         <v>VISUALSTUDIO: "Visual Studio",</v>
       </c>
     </row>
-    <row r="81" hidden="1" customHeight="1" spans="1:6">
+    <row r="81" customHeight="1" spans="1:6">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -3539,7 +3548,7 @@
         <v>SQLSERVER: "SQL Server",</v>
       </c>
     </row>
-    <row r="82" hidden="1" customHeight="1" spans="1:6">
+    <row r="82" customHeight="1" spans="1:6">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -3561,7 +3570,7 @@
         <v>VSCODE: "VSCode",</v>
       </c>
     </row>
-    <row r="83" hidden="1" customHeight="1" spans="1:6">
+    <row r="83" customHeight="1" spans="1:6">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -3583,7 +3592,7 @@
         <v>OFFICE: "Office",</v>
       </c>
     </row>
-    <row r="84" hidden="1" customHeight="1" spans="1:6">
+    <row r="84" customHeight="1" spans="1:6">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -3605,7 +3614,7 @@
         <v>GITLAB: "Gitlab",</v>
       </c>
     </row>
-    <row r="85" hidden="1" customHeight="1" spans="1:6">
+    <row r="85" customHeight="1" spans="1:6">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -3627,7 +3636,7 @@
         <v>LINUX: "Linux",</v>
       </c>
     </row>
-    <row r="86" hidden="1" customHeight="1" spans="1:6">
+    <row r="86" customHeight="1" spans="1:6">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -3649,7 +3658,7 @@
         <v>ANDROID: "Android",</v>
       </c>
     </row>
-    <row r="87" hidden="1" customHeight="1" spans="1:6">
+    <row r="87" customHeight="1" spans="1:6">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -3671,7 +3680,7 @@
         <v>APPLE: "Apple",</v>
       </c>
     </row>
-    <row r="88" hidden="1" customHeight="1" spans="1:6">
+    <row r="88" customHeight="1" spans="1:6">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -3693,7 +3702,7 @@
         <v>APPLE_IOS: "Apple iOS",</v>
       </c>
     </row>
-    <row r="89" hidden="1" customHeight="1" spans="1:6">
+    <row r="89" customHeight="1" spans="1:6">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -3715,7 +3724,7 @@
         <v>GOOGLE: "Google",</v>
       </c>
     </row>
-    <row r="90" hidden="1" customHeight="1" spans="1:6">
+    <row r="90" customHeight="1" spans="1:6">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -3737,7 +3746,7 @@
         <v>CHROME: "Chrome",</v>
       </c>
     </row>
-    <row r="91" hidden="1" customHeight="1" spans="1:6">
+    <row r="91" customHeight="1" spans="1:6">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -3759,7 +3768,7 @@
         <v>EDGE: "Microsoft Edge",</v>
       </c>
     </row>
-    <row r="92" hidden="1" customHeight="1" spans="1:6">
+    <row r="92" customHeight="1" spans="1:6">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -3781,7 +3790,7 @@
         <v>FIREFOX: "Firefox",</v>
       </c>
     </row>
-    <row r="93" hidden="1" customHeight="1" spans="1:6">
+    <row r="93" customHeight="1" spans="1:6">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -3803,7 +3812,7 @@
         <v>SAFARI: "Safari",</v>
       </c>
     </row>
-    <row r="94" hidden="1" customHeight="1" spans="1:6">
+    <row r="94" customHeight="1" spans="1:6">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -3825,7 +3834,7 @@
         <v>OFFICIAL_SITE: "Official Site",</v>
       </c>
     </row>
-    <row r="95" hidden="1" customHeight="1" spans="1:6">
+    <row r="95" customHeight="1" spans="1:6">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -3847,7 +3856,7 @@
         <v>EMAIL_ADDRESS: "Email Address",</v>
       </c>
     </row>
-    <row r="96" hidden="1" customHeight="1" spans="1:6">
+    <row r="96" customHeight="1" spans="1:6">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -3869,7 +3878,7 @@
         <v>TELEPHONE_NUMBER: "Telephone",</v>
       </c>
     </row>
-    <row r="97" hidden="1" customHeight="1" spans="1:6">
+    <row r="97" customHeight="1" spans="1:6">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -3891,7 +3900,7 @@
         <v>MOBILE_NUMBER: "Mobile Number",</v>
       </c>
     </row>
-    <row r="98" hidden="1" customHeight="1" spans="1:6">
+    <row r="98" customHeight="1" spans="1:6">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -3913,7 +3922,7 @@
         <v>USERNAME: "User Name",</v>
       </c>
     </row>
-    <row r="99" hidden="1" customHeight="1" spans="1:6">
+    <row r="99" customHeight="1" spans="1:6">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -3935,7 +3944,7 @@
         <v>PASSWORD: "Password",</v>
       </c>
     </row>
-    <row r="100" hidden="1" customHeight="1" spans="1:6">
+    <row r="100" customHeight="1" spans="1:6">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -3957,7 +3966,7 @@
         <v>REMEMBER_ME: "Remember Me",</v>
       </c>
     </row>
-    <row r="101" hidden="1" customHeight="1" spans="1:6">
+    <row r="101" customHeight="1" spans="1:6">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -3979,7 +3988,7 @@
         <v>AUTHENTICATE: "Authenticate",</v>
       </c>
     </row>
-    <row r="102" hidden="1" customHeight="1" spans="1:6">
+    <row r="102" customHeight="1" spans="1:6">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -4001,7 +4010,7 @@
         <v>APPLICATION_NAME: ".NET &amp; Vue",</v>
       </c>
     </row>
-    <row r="103" hidden="1" customHeight="1" spans="1:6">
+    <row r="103" customHeight="1" spans="1:6">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -4023,7 +4032,7 @@
         <v>CONTROL_PANEL: "Control Panel",</v>
       </c>
     </row>
-    <row r="104" hidden="1" customHeight="1" spans="1:6">
+    <row r="104" customHeight="1" spans="1:6">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -4045,7 +4054,7 @@
         <v>APPLICATION_MANIFEST: "Application Manifest",</v>
       </c>
     </row>
-    <row r="105" hidden="1" customHeight="1" spans="1:6">
+    <row r="105" customHeight="1" spans="1:6">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -4067,7 +4076,7 @@
         <v>INVALID_CREDENTIALS: "The username and login password must be provided.",</v>
       </c>
     </row>
-    <row r="106" hidden="1" customHeight="1" spans="1:6">
+    <row r="106" customHeight="1" spans="1:6">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -4089,7 +4098,7 @@
         <v>AUTHORIZE_FAILED: "Authorization failed.",</v>
       </c>
     </row>
-    <row r="107" hidden="1" customHeight="1" spans="1:6">
+    <row r="107" customHeight="1" spans="1:6">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -4111,7 +4120,7 @@
         <v>AUTHENTICATION_IN_PROGRESS: "Authentication in progress, please wait",</v>
       </c>
     </row>
-    <row r="108" hidden="1" customHeight="1" spans="1:6">
+    <row r="108" customHeight="1" spans="1:6">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -4133,7 +4142,7 @@
         <v>ENTER_USERNAME: "User Name / E-mail Address / Mobile Number",</v>
       </c>
     </row>
-    <row r="109" hidden="1" customHeight="1" spans="1:6">
+    <row r="109" customHeight="1" spans="1:6">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -4155,7 +4164,7 @@
         <v>ENTER_PASSWORD: "Password",</v>
       </c>
     </row>
-    <row r="110" hidden="1" customHeight="1" spans="1:6">
+    <row r="110" customHeight="1" spans="1:6">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -4177,7 +4186,7 @@
         <v>CURRENT_USER: "The user",</v>
       </c>
     </row>
-    <row r="111" hidden="1" customHeight="1" spans="1:6">
+    <row r="111" customHeight="1" spans="1:6">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -4199,15 +4208,30 @@
         <v>CHANGE_PASSWORD: "Change my password",</v>
       </c>
     </row>
+    <row r="112" customHeight="1" spans="1:6">
+      <c r="A112" s="4">
+        <v>111</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D112" s="2" t="str">
+        <f>UPPER(B112)&amp;": """&amp;C112&amp;""","</f>
+        <v>HOME_PAGE: "首页",</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F112" s="2" t="str">
+        <f>UPPER(B112)&amp;": """&amp;E112&amp;""","</f>
+        <v>HOME_PAGE: "Home",</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F111">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Expand"/>
-        <filter val="Next_Page"/>
-        <filter val="Exception"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A1:F112">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(Issue #17): 完善了 v-content-container.vue 组件。增加了通用加载中状态。
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="260">
   <si>
     <t>序号</t>
   </si>
@@ -788,6 +788,15 @@
   </si>
   <si>
     <t>Data Table</t>
+  </si>
+  <si>
+    <t>In_Processing</t>
+  </si>
+  <si>
+    <t>事务正在处理中，请稍候.....</t>
+  </si>
+  <si>
+    <t>The transaction is processing, please wait a few minutes...</t>
   </si>
 </sst>
 </file>
@@ -1758,12 +1767,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F112" sqref="F112:F113"/>
+      <selection pane="bottomLeft" activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -1772,8 +1781,8 @@
     <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="27.75" style="2" customWidth="1"/>
     <col min="4" max="4" width="57.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="45.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="63.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="49.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="68.875" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -4259,6 +4268,28 @@
       <c r="F113" s="2" t="str">
         <f>UPPER(B113)&amp;": """&amp;E113&amp;""","</f>
         <v>DATA_TABLE: "Data Table",</v>
+      </c>
+    </row>
+    <row r="114" customHeight="1" spans="1:6">
+      <c r="A114" s="4">
+        <v>113</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D114" s="2" t="str">
+        <f>UPPER(B114)&amp;": """&amp;C114&amp;""","</f>
+        <v>IN_PROCESSING: "事务正在处理中，请稍候.....",</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F114" s="2" t="str">
+        <f>UPPER(B114)&amp;": """&amp;E114&amp;""","</f>
+        <v>IN_PROCESSING: "The transaction is processing, please wait a few minutes...",</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 新增 v-btn.vue 组件。
调整 v-signin.vue 组件中的按钮。
</commit_message>
<xml_diff>
--- a/docs/i18n.xlsx
+++ b/docs/i18n.xlsx
@@ -10,14 +10,14 @@
     <sheet name="默认多语言资源" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">默认多语言资源!$A$1:$F$115</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="262">
   <si>
     <t>序号</t>
   </si>
@@ -797,6 +797,12 @@
   </si>
   <si>
     <t>The transaction is processing, please wait a few minutes...</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>按钮</t>
   </si>
 </sst>
 </file>
@@ -804,9 +810,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -838,15 +844,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -869,7 +866,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -882,9 +887,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,14 +918,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -937,25 +933,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -976,7 +974,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -991,7 +997,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1009,13 +1027,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,127 +1117,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1165,13 +1141,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1202,11 +1208,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1230,7 +1234,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1239,7 +1243,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1276,9 +1280,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1290,10 +1296,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1302,16 +1308,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1323,112 +1329,112 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1767,12 +1773,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F118" sqref="F118"/>
+      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
@@ -3841,14 +3847,14 @@
         <v>202</v>
       </c>
       <c r="D94" s="2" t="str">
-        <f t="shared" ref="D94:D112" si="14">UPPER(B94)&amp;": """&amp;C94&amp;""","</f>
+        <f t="shared" ref="D94:D114" si="14">UPPER(B94)&amp;": """&amp;C94&amp;""","</f>
         <v>OFFICIAL_SITE: "官网",</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>203</v>
       </c>
       <c r="F94" s="2" t="str">
-        <f t="shared" ref="F94:F112" si="15">UPPER(B94)&amp;": """&amp;E94&amp;""","</f>
+        <f t="shared" ref="F94:F114" si="15">UPPER(B94)&amp;": """&amp;E94&amp;""","</f>
         <v>OFFICIAL_SITE: "Official Site",</v>
       </c>
     </row>
@@ -4259,14 +4265,14 @@
         <v>255</v>
       </c>
       <c r="D113" s="2" t="str">
-        <f>UPPER(B113)&amp;": """&amp;C113&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>DATA_TABLE: "数据列表",</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>256</v>
       </c>
       <c r="F113" s="2" t="str">
-        <f>UPPER(B113)&amp;": """&amp;E113&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>DATA_TABLE: "Data Table",</v>
       </c>
     </row>
@@ -4281,19 +4287,41 @@
         <v>258</v>
       </c>
       <c r="D114" s="2" t="str">
-        <f>UPPER(B114)&amp;": """&amp;C114&amp;""","</f>
+        <f t="shared" si="14"/>
         <v>IN_PROCESSING: "事务正在处理中，请稍候.....",</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F114" s="2" t="str">
-        <f>UPPER(B114)&amp;": """&amp;E114&amp;""","</f>
+        <f t="shared" si="15"/>
         <v>IN_PROCESSING: "The transaction is processing, please wait a few minutes...",</v>
       </c>
     </row>
+    <row r="115" customHeight="1" spans="1:6">
+      <c r="A115" s="4">
+        <v>114</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D115" s="2" t="str">
+        <f>UPPER(B115)&amp;": """&amp;C115&amp;""","</f>
+        <v>BUTTON: "按钮",</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F115" s="2" t="str">
+        <f>UPPER(B115)&amp;": """&amp;E115&amp;""","</f>
+        <v>BUTTON: "Button",</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F112">
+  <autoFilter ref="A1:F115">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>